<commit_message>
Added test cases in to 1PRecommend
</commit_message>
<xml_diff>
--- a/src/test/test-data/RecommendTestData.xlsx
+++ b/src/test/test-data/RecommendTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>API</t>
   </si>
@@ -52,9 +52,6 @@
     <t>STORE</t>
   </si>
   <si>
-    <t>S1_TC_T1</t>
-  </si>
-  <si>
     <t>DEPENDENCYTESTS</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>?max=6</t>
   </si>
   <si>
-    <t>S1_TC_T2</t>
-  </si>
-  <si>
     <t>Verify that system is able to recommend articles for user</t>
   </si>
   <si>
@@ -83,13 +77,85 @@
   </si>
   <si>
     <t>?max=3</t>
+  </si>
+  <si>
+    <t>Verify that 1P-recommend API endpoint for article recommendations based on user selected documents</t>
+  </si>
+  <si>
+    <t>/recommend/debug/articles/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that 1P-recommend API endpoint to obtain total times cited for a given ORCID</t>
+  </si>
+  <si>
+    <t>/recommend/jcrmetrix=rid&amp;query=0000-0002-1553-596x</t>
+  </si>
+  <si>
+    <t>Verify that user should receive article recommendation on an article page</t>
+  </si>
+  <si>
+    <t>?source=articles&amp;fields=title</t>
+  </si>
+  <si>
+    <t>OPQA-896</t>
+  </si>
+  <si>
+    <t>Verify that to get articles for query</t>
+  </si>
+  <si>
+    <t>1PSEARCHV3</t>
+  </si>
+  <si>
+    <t>/wos/search</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1&amp;fields=citingsrcslocalcount&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>/recommend/matchingdocs/(OPQA-896_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>Verify that 1P-recommend API endpoint for predicted categories</t>
+  </si>
+  <si>
+    <t>/recommend/predict/biotechnology</t>
+  </si>
+  <si>
+    <t>hits.hits._id</t>
+  </si>
+  <si>
+    <t>/recommend/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that 1P-recommend API endpoint for recommending articles and peoples </t>
+  </si>
+  <si>
+    <t>OPQA-1103</t>
+  </si>
+  <si>
+    <t>OPQA-1102</t>
+  </si>
+  <si>
+    <t>OPQA-1399</t>
+  </si>
+  <si>
+    <t>OPQA-1400</t>
+  </si>
+  <si>
+    <t>OPQA-1401</t>
+  </si>
+  <si>
+    <t>OPQA-1402</t>
+  </si>
+  <si>
+    <t>OPQA-1403</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +170,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -144,10 +217,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -162,8 +239,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,15 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="44.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -504,7 +583,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
@@ -518,57 +597,197 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="45">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4"/>
+      <c r="J4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5"/>
+      <c r="J5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7"/>
+      <c r="J7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8"/>
+      <c r="J8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9"/>
+      <c r="J9" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>